<commit_message>
update Tuan1.md, Tuan1.tex and '#CaseStudy11-Lam sao de paste voi filter (BKIndex Group).xlsx'
</commit_message>
<xml_diff>
--- a/contents/Tuan1/Video5/#CaseStudy11-Lam sao de paste voi filter (BKIndex Group).xlsx
+++ b/contents/Tuan1/Video5/#CaseStudy11-Lam sao de paste voi filter (BKIndex Group).xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvn20206205\Desktop\Datawarehouse\contents\Tuan1\Video5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBBA617-A111-41BD-B047-259722B8F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yêu cầu" sheetId="2" r:id="rId1"/>
     <sheet name="Cách làm" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Cách làm'!$A$4:$D$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Cách làm'!$C$4:$D$11</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>band 1</t>
   </si>
@@ -149,12 +155,15 @@
   <si>
     <t>Sắp xếp vùng A4 đến D11 theo cột B</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -364,7 +373,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -426,7 +435,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo BKIndex.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="logo BKIndex.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -469,7 +484,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo BKIndex.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="logo BKIndex.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -750,27 +771,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="B3:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:12" ht="19.5" thickBot="1"/>
-    <row r="4" spans="2:12">
+    <row r="3" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -785,7 +806,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -800,7 +821,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -815,7 +836,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -830,7 +851,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -845,7 +866,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
@@ -860,7 +881,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
@@ -875,7 +896,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -890,7 +911,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
@@ -905,7 +926,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -918,7 +939,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="2:12" ht="19.5" thickBot="1">
+    <row r="14" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -931,8 +952,8 @@
       <c r="K14" s="8"/>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="2:12" ht="19.5" thickBot="1"/>
-    <row r="16" spans="2:12">
+    <row r="15" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
         <v>20</v>
       </c>
@@ -947,7 +968,7 @@
       <c r="K16" s="11"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="2:12" ht="19.5" thickBot="1">
+    <row r="17" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -967,34 +988,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0000CC"/>
   </sheetPr>
   <dimension ref="A2:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B6" sqref="B6:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" customWidth="1"/>
+    <col min="8" max="8" width="40.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H2" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H3" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.5" customHeight="1">
+    <row r="4" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="17" t="s">
         <v>5</v>
       </c>
@@ -1005,7 +1026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1019,15 +1040,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
       <c r="C6" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="16">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F6">
         <v>236</v>
@@ -1036,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1050,7 +1074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1064,7 +1088,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1078,15 +1102,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="37.5">
+    <row r="10" spans="1:8" ht="36" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
       <c r="C10" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -1095,7 +1122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1106,52 +1133,56 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H12" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H13" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H14" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H15" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H16" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="5:8">
+    <row r="17" spans="5:8" x14ac:dyDescent="0.35">
       <c r="H17" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="5:8">
+    <row r="18" spans="5:8" x14ac:dyDescent="0.35">
       <c r="H18" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="5:8">
+    <row r="19" spans="5:8" x14ac:dyDescent="0.35">
       <c r="H19" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="5:8">
+    <row r="22" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C4:D11" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:F11">
+    <sortCondition ref="A5:A11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>